<commit_message>
Add Page Options tests
* Add responsive test methods to TestRunner.
* Renamed breakpoints.
* Add `isVisible()` to `ElementHelper`.
</commit_message>
<xml_diff>
--- a/test-data/page-title-data.xlsx
+++ b/test-data/page-title-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/learnb/git/digiplat-qa/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci-repo\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741314E5-CFFF-224A-AE2B-D6D6FFAB2E08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12F3905-9A1B-459D-8034-B4AFFD7C6F6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="4380" windowWidth="27640" windowHeight="16940" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="11625" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="browser_and_page_titles" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>path</t>
   </si>
@@ -41,30 +41,18 @@
     <t>language</t>
   </si>
   <si>
-    <t>about-cancer/coping/feelings</t>
-  </si>
-  <si>
     <t>Article</t>
   </si>
   <si>
     <t>English</t>
   </si>
   <si>
-    <t>/espanol/node/1</t>
-  </si>
-  <si>
     <t>Spanish</t>
   </si>
   <si>
     <t>/about-cancer/coping/feelings/relaxation</t>
   </si>
   <si>
-    <t>/espanol/node/6</t>
-  </si>
-  <si>
-    <t>/node/36</t>
-  </si>
-  <si>
     <t>Cancer Center</t>
   </si>
   <si>
@@ -80,12 +68,6 @@
     <t xml:space="preserve">Feelings and Cancer </t>
   </si>
   <si>
-    <t>Los sentimientos y el cáncer | CGDP - Dev</t>
-  </si>
-  <si>
-    <t>Los sentimientos y el cáncer</t>
-  </si>
-  <si>
     <t>Learning to Relax | CGDP - Dev</t>
   </si>
   <si>
@@ -98,23 +80,50 @@
     <t>Aprenda a relajarse</t>
   </si>
   <si>
-    <t>Duke Cancer Center | CGDP - Dev</t>
-  </si>
-  <si>
-    <t>Duke Cancer Center</t>
+    <t>/about-cancer/coping/feelings/relaxation/dfharvard</t>
+  </si>
+  <si>
+    <t>Dana Farber/Harvard Cancer Center | CGDP - Dev</t>
+  </si>
+  <si>
+    <t>Dana Farber/Harvard Cancer Center</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/loukissas-jennifer</t>
+  </si>
+  <si>
+    <t>Biography</t>
+  </si>
+  <si>
+    <t>Jennifer K. Loukissas, M.P.P.</t>
+  </si>
+  <si>
+    <t>Jennifer K. Loukissas, M.P.P. | CGDP - Dev</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/sobrellevar/sentimientos/relajarse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,17 +465,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,98 +488,99 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(#12)Added tests for PageTitle
</commit_message>
<xml_diff>
--- a/test-data/page-title-data.xlsx
+++ b/test-data/page-title-data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci-repo\cgov-digital-platform-qa\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12F3905-9A1B-459D-8034-B4AFFD7C6F6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3290E997-FC5D-43AB-A2DC-E6B476C3A1C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="11625" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
-    <sheet name="browser_and_page_titles" sheetId="1" r:id="rId1"/>
+    <sheet name="page_title" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>path</t>
   </si>
@@ -56,36 +56,15 @@
     <t>Cancer Center</t>
   </si>
   <si>
-    <t>browser_title</t>
-  </si>
-  <si>
-    <t>content_title</t>
-  </si>
-  <si>
-    <t>Feelings and Cancer | CGDP - Dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feelings and Cancer </t>
-  </si>
-  <si>
-    <t>Learning to Relax | CGDP - Dev</t>
-  </si>
-  <si>
     <t>Learning to Relax</t>
   </si>
   <si>
-    <t>Aprenda a relajarse | CGDP - Dev</t>
-  </si>
-  <si>
     <t>Aprenda a relajarse</t>
   </si>
   <si>
     <t>/about-cancer/coping/feelings/relaxation/dfharvard</t>
   </si>
   <si>
-    <t>Dana Farber/Harvard Cancer Center | CGDP - Dev</t>
-  </si>
-  <si>
     <t>Dana Farber/Harvard Cancer Center</t>
   </si>
   <si>
@@ -98,13 +77,52 @@
     <t>Jennifer K. Loukissas, M.P.P.</t>
   </si>
   <si>
-    <t>Jennifer K. Loukissas, M.P.P. | CGDP - Dev</t>
-  </si>
-  <si>
     <t>/about-cancer/coping/feelings</t>
   </si>
   <si>
     <t>/espanol/cancer/sobrellevar/sentimientos/relajarse</t>
+  </si>
+  <si>
+    <t>page_title</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/sobrellevar/sentimientos</t>
+  </si>
+  <si>
+    <t>Los sentimientos y el cáncer</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog/2019/vitamin-d-supplement-cancer-prevention</t>
+  </si>
+  <si>
+    <t>Vitamin D Supplements Don’t Reduce Cancer Incidence, Trial Shows</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/temas-y-relatos-blog/2019/vitamina-d-complemento-cancer-prevencion</t>
+  </si>
+  <si>
+    <t>Estudio indica que complementos de vitamina D no reducen la incidencia de cáncer</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/comunicados-de-prensa/2018/leucemia-llc-ibrutinib-estudio</t>
+  </si>
+  <si>
+    <t>Press Release</t>
+  </si>
+  <si>
+    <t>Leucemia - Ibrutinib más rituximab fue superior al tratamiento convencional para algunos pacientes con leucemia linfocítica crónica</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018/leukemia-cll-ibrutinib-trial</t>
+  </si>
+  <si>
+    <t>Leukemia - Ibrutinib plus rituximab superior to standard treatment for some patients with chronic leukemia</t>
+  </si>
+  <si>
+    <t>Feelings and Cancer</t>
   </si>
 </sst>
 </file>
@@ -463,21 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="49.9140625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,15 +505,12 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -505,15 +519,12 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -522,61 +533,119 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>